<commit_message>
User submitted updates content changes
Changes made to content and dams template based on team discussion.
</commit_message>
<xml_diff>
--- a/docs/source/docs_user/downloads/damstemplate4202022.xlsx
+++ b/docs/source/docs_user/downloads/damstemplate4202022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\Documentation\docs\source\docs_user\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBE4809-423E-4148-AEB2-D47B6356BFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A12FA49-A24E-4115-995E-3B3E0A3DFCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19640" yWindow="150" windowWidth="31980" windowHeight="19500" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
   </bookViews>
   <sheets>
     <sheet name="new_data" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="dam_condition">field_list!$B$9:$E$9</definedName>
     <definedName name="dam_use">field_list!$B$12:$L$12</definedName>
     <definedName name="down_passage_route">field_list!$B$14:$E$14</definedName>
+    <definedName name="entry_classification">field_list!$B$62:$D$62</definedName>
     <definedName name="function_name">field_list!$B$20:$N$20</definedName>
     <definedName name="lake_control">field_list!$B$24:$D$24</definedName>
     <definedName name="operating_status">field_list!$B$30:$F$30</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="144">
   <si>
     <t>cabd_id</t>
   </si>
@@ -483,6 +484,18 @@
   </si>
   <si>
     <t>secondary</t>
+  </si>
+  <si>
+    <t>delete feature</t>
+  </si>
+  <si>
+    <t>modify feature</t>
+  </si>
+  <si>
+    <t>new feature</t>
+  </si>
+  <si>
+    <t>entry_classification</t>
   </si>
 </sst>
 </file>
@@ -863,7 +876,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0988C4D-359E-42BE-924C-BF04784F7938}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -871,29 +884,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" customWidth="1"/>
-    <col min="4" max="4" width="66.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" customWidth="1"/>
+    <col min="5" max="5" width="66.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="27" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="F1" s="5" t="s">
         <v>64</v>
       </c>
@@ -957,197 +971,203 @@
       <c r="Z1" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B2" s="3"/>
+      <c r="AA1" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B4" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B5" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B6" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B10" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B11" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B12" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B13" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B15" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B16" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="27">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51:F99" xr:uid="{5AF37559-2629-420A-98F2-B2DA443BA8C9}">
+  <dataValidations count="28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51:G99" xr:uid="{5AF37559-2629-420A-98F2-B2DA443BA8C9}">
+      <formula1>INDIRECT($G$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51:F99" xr:uid="{1667F174-C0D1-425D-AE1E-FA0641E2ADB3}">
       <formula1>INDIRECT($F$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E51:E99" xr:uid="{1667F174-C0D1-425D-AE1E-FA0641E2ADB3}">
-      <formula1>INDIRECT($E$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51:G99" xr:uid="{89498156-E0C9-4734-B941-966465F4E7B2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51:H99" xr:uid="{89498156-E0C9-4734-B941-966465F4E7B2}">
+      <formula1>INDIRECT($H$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J51:AA99" xr:uid="{F36B32A2-2B7E-47AF-A769-545AF0847515}">
+      <formula1>INDIRECT(J50)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51:I99" xr:uid="{4BB39194-6EB9-4960-B312-C170FAE496C3}">
+      <formula1>INDIRECT($I$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="J2:J50" xr:uid="{ABAE0820-5601-4115-BB9C-31E9E6D9AF54}">
+      <formula1>INDIRECT($J$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="K2:K50" xr:uid="{DEE68547-BBAA-49EF-85A7-E3B7128EAF45}">
+      <formula1>INDIRECT($K$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="L2:L50" xr:uid="{DD26ED87-4654-488E-AE8B-EAE054004B9C}">
+      <formula1>INDIRECT($L$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="M2:M50" xr:uid="{9BC55E85-0FA8-4843-BE1E-99586420BE8E}">
+      <formula1>INDIRECT($M$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="N2:N50" xr:uid="{AC179DE8-166A-48E9-99F7-5BA47AAC62BC}">
+      <formula1>INDIRECT($N$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="O2:O50" xr:uid="{4D7E8F93-CE36-4DD9-A3EB-7DDE622D55C9}">
+      <formula1>INDIRECT($O$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="P2:P50" xr:uid="{A6D76EA0-E6E8-46F0-8FC7-566717DE4009}">
+      <formula1>INDIRECT($P$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="Q2:Q50" xr:uid="{C3DCC9F0-E06A-410A-BC2A-BEB7F833CA9B}">
+      <formula1>INDIRECT($Q$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="R2:R50" xr:uid="{8E920611-53C4-4E32-86C4-B20AFB087A04}">
+      <formula1>INDIRECT($R$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="S2:S50" xr:uid="{BF444A8F-3692-4C22-B7D5-9AC749B4D7FE}">
+      <formula1>INDIRECT($S$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="T2:T50" xr:uid="{C1A61043-7610-49B6-9799-3875AC39BD2A}">
+      <formula1>INDIRECT($T$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="U2:U50" xr:uid="{218A845F-8394-47AF-AC54-101C807B51FC}">
+      <formula1>INDIRECT($U$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="V2:V50" xr:uid="{8EFA96F0-5548-45A0-A523-913170CC7959}">
+      <formula1>INDIRECT($V$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="W2:W50" xr:uid="{41F7CE9D-4670-4F45-9E54-5F36F4F37FEA}">
+      <formula1>INDIRECT($W$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="X2:X50" xr:uid="{7A498021-8BA2-438B-A0FA-6076D41A1C26}">
+      <formula1>INDIRECT($X$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="Y2:Y50" xr:uid="{D57F7E8B-25BF-4E92-BF75-FE37F82F0FCE}">
+      <formula1>INDIRECT($Y$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="Z2:Z50" xr:uid="{9E15A899-8A58-4726-B9DA-814FA8FBDF7C}">
+      <formula1>INDIRECT($Z$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="AA2:AA50" xr:uid="{F41BE7BF-057E-4E3B-9E9C-C8B7AFA9DA5E}">
+      <formula1>INDIRECT($AA$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F2:F50" xr:uid="{19A27413-45A8-4D3C-ABDD-44A91BA18C61}">
+      <formula1>INDIRECT($F$1)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="G2:G50" xr:uid="{E51777D1-078F-43BA-B3B9-474EA7F07003}">
       <formula1>INDIRECT($G$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I51:Z99" xr:uid="{F36B32A2-2B7E-47AF-A769-545AF0847515}">
-      <formula1>INDIRECT(I50)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51:H99" xr:uid="{4BB39194-6EB9-4960-B312-C170FAE496C3}">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H50" xr:uid="{06B96DC9-60F7-419A-A173-9F661210FCE4}">
       <formula1>INDIRECT($H$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I50" xr:uid="{ABAE0820-5601-4115-BB9C-31E9E6D9AF54}">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I50" xr:uid="{C55D9A37-109A-4704-8B4A-02541C04258F}">
       <formula1>INDIRECT($I$1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J50" xr:uid="{DEE68547-BBAA-49EF-85A7-E3B7128EAF45}">
-      <formula1>INDIRECT($J$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K2:K50" xr:uid="{DD26ED87-4654-488E-AE8B-EAE054004B9C}">
-      <formula1>INDIRECT($K$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="L2:L50" xr:uid="{9BC55E85-0FA8-4843-BE1E-99586420BE8E}">
-      <formula1>INDIRECT($L$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="M2:M50" xr:uid="{AC179DE8-166A-48E9-99F7-5BA47AAC62BC}">
-      <formula1>INDIRECT($M$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="N2:N50" xr:uid="{4D7E8F93-CE36-4DD9-A3EB-7DDE622D55C9}">
-      <formula1>INDIRECT($N$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="O2:O50" xr:uid="{A6D76EA0-E6E8-46F0-8FC7-566717DE4009}">
-      <formula1>INDIRECT($O$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="P2:P50" xr:uid="{C3DCC9F0-E06A-410A-BC2A-BEB7F833CA9B}">
-      <formula1>INDIRECT($P$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Q2:Q50" xr:uid="{8E920611-53C4-4E32-86C4-B20AFB087A04}">
-      <formula1>INDIRECT($Q$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="R2:R50" xr:uid="{BF444A8F-3692-4C22-B7D5-9AC749B4D7FE}">
-      <formula1>INDIRECT($R$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="S2:S50" xr:uid="{C1A61043-7610-49B6-9799-3875AC39BD2A}">
-      <formula1>INDIRECT($S$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="T2:T50" xr:uid="{218A845F-8394-47AF-AC54-101C807B51FC}">
-      <formula1>INDIRECT($T$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="U2:U50" xr:uid="{8EFA96F0-5548-45A0-A523-913170CC7959}">
-      <formula1>INDIRECT($U$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="V2:V50" xr:uid="{41F7CE9D-4670-4F45-9E54-5F36F4F37FEA}">
-      <formula1>INDIRECT($V$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="W2:W50" xr:uid="{7A498021-8BA2-438B-A0FA-6076D41A1C26}">
-      <formula1>INDIRECT($W$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="X2:X50" xr:uid="{D57F7E8B-25BF-4E92-BF75-FE37F82F0FCE}">
-      <formula1>INDIRECT($X$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Y2:Y50" xr:uid="{9E15A899-8A58-4726-B9DA-814FA8FBDF7C}">
-      <formula1>INDIRECT($Y$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Z2:Z50" xr:uid="{F41BE7BF-057E-4E3B-9E9C-C8B7AFA9DA5E}">
-      <formula1>INDIRECT($Z$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E50" xr:uid="{19A27413-45A8-4D3C-ABDD-44A91BA18C61}">
-      <formula1>INDIRECT($E$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F50" xr:uid="{E51777D1-078F-43BA-B3B9-474EA7F07003}">
-      <formula1>INDIRECT($F$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G50" xr:uid="{06B96DC9-60F7-419A-A173-9F661210FCE4}">
-      <formula1>INDIRECT($G$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H2:H50" xr:uid="{C55D9A37-109A-4704-8B4A-02541C04258F}">
-      <formula1>INDIRECT($H$1)</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="A2:A50" xr:uid="{67A977D0-365A-4738-95B0-232CBEB5B488}">
+      <formula1>INDIRECT($A$1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1159,7 +1179,7 @@
           <x14:formula1>
             <xm:f>field_list!$A$2:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:Z1</xm:sqref>
+          <xm:sqref>F1:AA1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1170,10 +1190,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF453082-EDAE-48A4-8650-E89344D67BEF}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1838,14 +1858,37 @@
         <v>63</v>
       </c>
     </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="d8vZgoT40RHld8EgAPWct1P3eUfe+qWdKNp3CguZtrwyIJE35Et0+hzEG1zWmNlmEtziJphhlJ8yTWSHFR7k4Q==" saltValue="aozBatrr7eVu4uLKsmKofg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F2D6C6860AC114F8559403465E77CC4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9aa0fab731e12ae43c9a80a3688a0dbb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="411171ba-2276-4762-a69b-ae0a1d76a912" xmlns:ns3="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f403611b0be061c7eaebfc49762584e" ns2:_="" ns3:_="">
     <xsd:import namespace="411171ba-2276-4762-a69b-ae0a1d76a912"/>
@@ -2068,15 +2111,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2084,6 +2118,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE4609A-9376-4E3F-8C1A-0281507B16A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6B6A510-FC8E-43E9-B08C-E3DE3110F8A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2098,14 +2140,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE4609A-9376-4E3F-8C1A-0281507B16A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>